<commit_message>
Computer folder structure and github backup system set.
</commit_message>
<xml_diff>
--- a/Hours_Report/Hours spent_2024QB.xlsx
+++ b/Hours_Report/Hours spent_2024QB.xlsx
@@ -640,7 +640,7 @@
   <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -654,7 +654,7 @@
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E1" s="14">
         <f>SUM(D:D)</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F1" s="14" t="s">
         <v>38</v>
@@ -690,11 +690,11 @@
         <v>45503</v>
       </c>
       <c r="B4" s="12">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D4" s="11">
         <f t="shared" ref="D4:D39" si="0">+SUM(B4:C4)</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E4" t="s">
         <v>39</v>

</xml_diff>